<commit_message>
nop file schedule tuan 4
</commit_message>
<xml_diff>
--- a/_tainh/ReactJS_Training_Schedule.xlsx
+++ b/_tainh/ReactJS_Training_Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\May_tai\Du_Lieu\HK6\Thuc tap\report\Intership\_tainh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AB030B-0042-48C7-B874-886ECDC1B177}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED94C3A3-67BF-4D14-9F3E-A3578366987B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendant List" sheetId="5" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="114">
   <si>
     <t>Training Outline</t>
   </si>
@@ -407,9 +408,6 @@
   </si>
   <si>
     <t>80/100</t>
-  </si>
-  <si>
-    <t>11/072/109</t>
   </si>
   <si>
     <t>90/100</t>
@@ -859,6 +857,30 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -868,31 +890,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4536,8 +4534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5441,10 +5439,10 @@
       </c>
     </row>
     <row r="8" spans="2:12" s="1" customFormat="1" ht="51" customHeight="1">
-      <c r="B8" s="81">
+      <c r="B8" s="80">
         <v>3</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="77" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -5454,10 +5452,10 @@
         <v>8</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="83" t="s">
         <v>27</v>
       </c>
       <c r="I8" s="12">
@@ -5474,8 +5472,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" s="1" customFormat="1">
-      <c r="B9" s="82"/>
-      <c r="C9" s="79"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="78"/>
       <c r="D9" s="8" t="s">
         <v>44</v>
       </c>
@@ -5483,8 +5481,8 @@
         <v>8</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="76"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="84"/>
       <c r="I9" s="12">
         <v>43641</v>
       </c>
@@ -5499,8 +5497,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" s="1" customFormat="1">
-      <c r="B10" s="82"/>
-      <c r="C10" s="79"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="78"/>
       <c r="D10" s="8" t="s">
         <v>45</v>
       </c>
@@ -5508,8 +5506,8 @@
         <v>8</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="76"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="84"/>
       <c r="I10" s="12">
         <v>43641</v>
       </c>
@@ -5524,8 +5522,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" s="1" customFormat="1" ht="51">
-      <c r="B11" s="82"/>
-      <c r="C11" s="79"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="8" t="s">
         <v>49</v>
       </c>
@@ -5533,8 +5531,8 @@
         <v>8</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="76"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="84"/>
       <c r="I11" s="12">
         <v>43642</v>
       </c>
@@ -5549,8 +5547,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" s="1" customFormat="1">
-      <c r="B12" s="82"/>
-      <c r="C12" s="79"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="8" t="s">
         <v>47</v>
       </c>
@@ -5558,8 +5556,8 @@
         <v>8</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="76"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="84"/>
       <c r="I12" s="12">
         <v>43642</v>
       </c>
@@ -5574,8 +5572,8 @@
       </c>
     </row>
     <row r="13" spans="2:12" s="1" customFormat="1">
-      <c r="B13" s="83"/>
-      <c r="C13" s="80"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="62" t="s">
         <v>102</v>
       </c>
@@ -5583,18 +5581,18 @@
         <v>2</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="76"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="84"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="49"/>
     </row>
     <row r="14" spans="2:12" s="1" customFormat="1">
-      <c r="B14" s="81">
+      <c r="B14" s="80">
         <v>4</v>
       </c>
-      <c r="C14" s="84" t="s">
+      <c r="C14" s="75" t="s">
         <v>60</v>
       </c>
       <c r="D14" s="15" t="s">
@@ -5604,10 +5602,10 @@
         <v>8</v>
       </c>
       <c r="F14" s="15"/>
-      <c r="G14" s="78" t="s">
+      <c r="G14" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="H14" s="76"/>
+      <c r="H14" s="84"/>
       <c r="I14" s="12">
         <v>43647</v>
       </c>
@@ -5622,8 +5620,8 @@
       </c>
     </row>
     <row r="15" spans="2:12" s="1" customFormat="1">
-      <c r="B15" s="82"/>
-      <c r="C15" s="85"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="86"/>
       <c r="D15" s="15" t="s">
         <v>64</v>
       </c>
@@ -5631,8 +5629,8 @@
         <v>8</v>
       </c>
       <c r="F15" s="15"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="76"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="84"/>
       <c r="I15" s="12">
         <v>43648</v>
       </c>
@@ -5647,8 +5645,8 @@
       </c>
     </row>
     <row r="16" spans="2:12" s="1" customFormat="1">
-      <c r="B16" s="82"/>
-      <c r="C16" s="85"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="86"/>
       <c r="D16" s="15" t="s">
         <v>66</v>
       </c>
@@ -5656,8 +5654,8 @@
         <v>8</v>
       </c>
       <c r="F16" s="15"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="76"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="84"/>
       <c r="I16" s="12">
         <v>43648</v>
       </c>
@@ -5672,8 +5670,8 @@
       </c>
     </row>
     <row r="17" spans="2:12" s="1" customFormat="1">
-      <c r="B17" s="82"/>
-      <c r="C17" s="85"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="86"/>
       <c r="D17" s="15" t="s">
         <v>68</v>
       </c>
@@ -5681,8 +5679,8 @@
         <v>8</v>
       </c>
       <c r="F17" s="15"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="76"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="84"/>
       <c r="I17" s="12">
         <v>43648</v>
       </c>
@@ -5690,15 +5688,15 @@
         <v>43649</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L17" s="7" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="2:12" s="1" customFormat="1">
-      <c r="B18" s="82"/>
-      <c r="C18" s="85"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="86"/>
       <c r="D18" s="15" t="s">
         <v>70</v>
       </c>
@@ -5706,8 +5704,8 @@
         <v>8</v>
       </c>
       <c r="F18" s="15"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="76"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="84"/>
       <c r="I18" s="12">
         <v>43650</v>
       </c>
@@ -5722,8 +5720,8 @@
       </c>
     </row>
     <row r="19" spans="2:12" s="1" customFormat="1">
-      <c r="B19" s="82"/>
-      <c r="C19" s="85"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="86"/>
       <c r="D19" s="15" t="s">
         <v>72</v>
       </c>
@@ -5731,8 +5729,8 @@
         <v>8</v>
       </c>
       <c r="F19" s="15"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="76"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="84"/>
       <c r="I19" s="12">
         <v>43651</v>
       </c>
@@ -5740,15 +5738,15 @@
         <v>43651</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L19" s="7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="20" spans="2:12" s="1" customFormat="1">
-      <c r="B20" s="82"/>
-      <c r="C20" s="85"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="86"/>
       <c r="D20" s="15" t="s">
         <v>74</v>
       </c>
@@ -5756,8 +5754,8 @@
         <v>8</v>
       </c>
       <c r="F20" s="15"/>
-      <c r="G20" s="79"/>
-      <c r="H20" s="76"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="84"/>
       <c r="I20" s="12">
         <v>43654</v>
       </c>
@@ -5765,15 +5763,15 @@
         <v>43654</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L20" s="7" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:12" s="1" customFormat="1">
-      <c r="B21" s="82"/>
-      <c r="C21" s="85"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="15" t="s">
         <v>76</v>
       </c>
@@ -5781,8 +5779,8 @@
         <v>16</v>
       </c>
       <c r="F21" s="15"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="76"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="84"/>
       <c r="I21" s="12">
         <v>43654</v>
       </c>
@@ -5797,8 +5795,8 @@
       </c>
     </row>
     <row r="22" spans="2:12" s="1" customFormat="1">
-      <c r="B22" s="82"/>
-      <c r="C22" s="85"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="86"/>
       <c r="D22" s="15" t="s">
         <v>78</v>
       </c>
@@ -5806,8 +5804,8 @@
         <v>16</v>
       </c>
       <c r="F22" s="15"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="76"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="84"/>
       <c r="I22" s="12">
         <v>43655</v>
       </c>
@@ -5822,8 +5820,8 @@
       </c>
     </row>
     <row r="23" spans="2:12" s="1" customFormat="1">
-      <c r="B23" s="82"/>
-      <c r="C23" s="85"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="86"/>
       <c r="D23" s="15" t="s">
         <v>80</v>
       </c>
@@ -5831,8 +5829,8 @@
         <v>16</v>
       </c>
       <c r="F23" s="15"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="76"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="84"/>
       <c r="I23" s="12">
         <v>43655</v>
       </c>
@@ -5840,15 +5838,15 @@
         <v>43655</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L23" s="7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="24" spans="2:12" s="1" customFormat="1" ht="25.5">
-      <c r="B24" s="82"/>
-      <c r="C24" s="85"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="86"/>
       <c r="D24" s="15" t="s">
         <v>82</v>
       </c>
@@ -5856,8 +5854,8 @@
         <v>20</v>
       </c>
       <c r="F24" s="15"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="76"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="84"/>
       <c r="I24" s="12">
         <v>43656</v>
       </c>
@@ -5872,8 +5870,8 @@
       </c>
     </row>
     <row r="25" spans="2:12" s="1" customFormat="1">
-      <c r="B25" s="82"/>
-      <c r="C25" s="85"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="86"/>
       <c r="D25" s="15" t="s">
         <v>84</v>
       </c>
@@ -5881,13 +5879,13 @@
         <v>20</v>
       </c>
       <c r="F25" s="15"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="77"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="85"/>
       <c r="I25" s="12">
         <v>43657</v>
       </c>
-      <c r="J25" s="12" t="s">
-        <v>113</v>
+      <c r="J25" s="12">
+        <v>43657</v>
       </c>
       <c r="K25" s="12" t="s">
         <v>112</v>
@@ -5897,8 +5895,8 @@
       </c>
     </row>
     <row r="26" spans="2:12" s="1" customFormat="1">
-      <c r="B26" s="82"/>
-      <c r="C26" s="86"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="76"/>
       <c r="D26" s="62" t="s">
         <v>108</v>
       </c>
@@ -5906,7 +5904,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="15"/>
-      <c r="G26" s="80"/>
+      <c r="G26" s="79"/>
       <c r="H26" s="57"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5914,10 +5912,10 @@
       <c r="L26" s="7"/>
     </row>
     <row r="27" spans="2:12" s="1" customFormat="1" ht="38.25">
-      <c r="B27" s="82">
+      <c r="B27" s="81">
         <v>5</v>
       </c>
-      <c r="C27" s="84" t="s">
+      <c r="C27" s="75" t="s">
         <v>86</v>
       </c>
       <c r="D27" s="44" t="s">
@@ -5927,20 +5925,26 @@
         <v>50</v>
       </c>
       <c r="F27" s="15"/>
-      <c r="G27" s="78" t="s">
+      <c r="G27" s="77" t="s">
         <v>88</v>
       </c>
       <c r="H27" s="53"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="I27" s="12">
+        <v>43661</v>
+      </c>
+      <c r="J27" s="12">
+        <v>43664</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="L27" s="50" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="28" spans="2:12" s="1" customFormat="1">
-      <c r="B28" s="83"/>
-      <c r="C28" s="86"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="76"/>
       <c r="D28" s="62" t="s">
         <v>109</v>
       </c>
@@ -5948,7 +5952,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="15"/>
-      <c r="G28" s="80"/>
+      <c r="G28" s="79"/>
       <c r="H28" s="57"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -6035,12 +6039,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="G14:G26"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="B14:B26"/>
-    <mergeCell ref="B27:B28"/>
     <mergeCell ref="H8:H25"/>
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="B8:B13"/>
@@ -6056,6 +6054,12 @@
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="L4:L5"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="G14:G26"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="B14:B26"/>
+    <mergeCell ref="B27:B28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L8" r:id="rId1" display="https://www.w3schools.com/js/default.asp" xr:uid="{00000000-0004-0000-0400-000000000000}"/>

</xml_diff>

<commit_message>
nop file schedule tuan 5
</commit_message>
<xml_diff>
--- a/_tainh/ReactJS_Training_Schedule.xlsx
+++ b/_tainh/ReactJS_Training_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\May_tai\Du_Lieu\HK6\Thuc tap\report\Intership\_tainh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED94C3A3-67BF-4D14-9F3E-A3578366987B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37FD1D2-03E9-494F-B855-252B119AC844}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="112">
   <si>
     <t>Training Outline</t>
   </si>
@@ -402,12 +402,6 @@
   </si>
   <si>
     <t>100/100</t>
-  </si>
-  <si>
-    <t>70/100</t>
-  </si>
-  <si>
-    <t>80/100</t>
   </si>
   <si>
     <t>90/100</t>
@@ -857,40 +851,40 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4534,8 +4528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5432,17 +5426,17 @@
         <v>43670</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L7" s="48" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:12" s="1" customFormat="1" ht="51" customHeight="1">
-      <c r="B8" s="80">
+      <c r="B8" s="81">
         <v>3</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="78" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -5452,10 +5446,10 @@
         <v>8</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="77" t="s">
+      <c r="G8" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="83" t="s">
+      <c r="H8" s="75" t="s">
         <v>27</v>
       </c>
       <c r="I8" s="12">
@@ -5472,8 +5466,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" s="1" customFormat="1">
-      <c r="B9" s="81"/>
-      <c r="C9" s="78"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="79"/>
       <c r="D9" s="8" t="s">
         <v>44</v>
       </c>
@@ -5481,8 +5475,8 @@
         <v>8</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="84"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
       <c r="I9" s="12">
         <v>43641</v>
       </c>
@@ -5497,8 +5491,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" s="1" customFormat="1">
-      <c r="B10" s="81"/>
-      <c r="C10" s="78"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="79"/>
       <c r="D10" s="8" t="s">
         <v>45</v>
       </c>
@@ -5506,8 +5500,8 @@
         <v>8</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="84"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
       <c r="I10" s="12">
         <v>43641</v>
       </c>
@@ -5522,8 +5516,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" s="1" customFormat="1" ht="51">
-      <c r="B11" s="81"/>
-      <c r="C11" s="78"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="8" t="s">
         <v>49</v>
       </c>
@@ -5531,8 +5525,8 @@
         <v>8</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="84"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
       <c r="I11" s="12">
         <v>43642</v>
       </c>
@@ -5547,8 +5541,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" s="1" customFormat="1">
-      <c r="B12" s="81"/>
-      <c r="C12" s="78"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="8" t="s">
         <v>47</v>
       </c>
@@ -5556,8 +5550,8 @@
         <v>8</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="84"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="76"/>
       <c r="I12" s="12">
         <v>43642</v>
       </c>
@@ -5572,8 +5566,8 @@
       </c>
     </row>
     <row r="13" spans="2:12" s="1" customFormat="1">
-      <c r="B13" s="82"/>
-      <c r="C13" s="79"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="62" t="s">
         <v>102</v>
       </c>
@@ -5581,18 +5575,18 @@
         <v>2</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="76"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="49"/>
     </row>
     <row r="14" spans="2:12" s="1" customFormat="1">
-      <c r="B14" s="80">
+      <c r="B14" s="81">
         <v>4</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="84" t="s">
         <v>60</v>
       </c>
       <c r="D14" s="15" t="s">
@@ -5602,10 +5596,10 @@
         <v>8</v>
       </c>
       <c r="F14" s="15"/>
-      <c r="G14" s="77" t="s">
+      <c r="G14" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="H14" s="84"/>
+      <c r="H14" s="76"/>
       <c r="I14" s="12">
         <v>43647</v>
       </c>
@@ -5620,8 +5614,8 @@
       </c>
     </row>
     <row r="15" spans="2:12" s="1" customFormat="1">
-      <c r="B15" s="81"/>
-      <c r="C15" s="86"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="15" t="s">
         <v>64</v>
       </c>
@@ -5629,8 +5623,8 @@
         <v>8</v>
       </c>
       <c r="F15" s="15"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="84"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="76"/>
       <c r="I15" s="12">
         <v>43648</v>
       </c>
@@ -5645,8 +5639,8 @@
       </c>
     </row>
     <row r="16" spans="2:12" s="1" customFormat="1">
-      <c r="B16" s="81"/>
-      <c r="C16" s="86"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="15" t="s">
         <v>66</v>
       </c>
@@ -5654,8 +5648,8 @@
         <v>8</v>
       </c>
       <c r="F16" s="15"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="84"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="76"/>
       <c r="I16" s="12">
         <v>43648</v>
       </c>
@@ -5670,8 +5664,8 @@
       </c>
     </row>
     <row r="17" spans="2:12" s="1" customFormat="1">
-      <c r="B17" s="81"/>
-      <c r="C17" s="86"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="15" t="s">
         <v>68</v>
       </c>
@@ -5679,8 +5673,8 @@
         <v>8</v>
       </c>
       <c r="F17" s="15"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="84"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="76"/>
       <c r="I17" s="12">
         <v>43648</v>
       </c>
@@ -5695,8 +5689,8 @@
       </c>
     </row>
     <row r="18" spans="2:12" s="1" customFormat="1">
-      <c r="B18" s="81"/>
-      <c r="C18" s="86"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="15" t="s">
         <v>70</v>
       </c>
@@ -5704,8 +5698,8 @@
         <v>8</v>
       </c>
       <c r="F18" s="15"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="84"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="76"/>
       <c r="I18" s="12">
         <v>43650</v>
       </c>
@@ -5720,8 +5714,8 @@
       </c>
     </row>
     <row r="19" spans="2:12" s="1" customFormat="1">
-      <c r="B19" s="81"/>
-      <c r="C19" s="86"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="15" t="s">
         <v>72</v>
       </c>
@@ -5729,8 +5723,8 @@
         <v>8</v>
       </c>
       <c r="F19" s="15"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="84"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="76"/>
       <c r="I19" s="12">
         <v>43651</v>
       </c>
@@ -5745,8 +5739,8 @@
       </c>
     </row>
     <row r="20" spans="2:12" s="1" customFormat="1">
-      <c r="B20" s="81"/>
-      <c r="C20" s="86"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="15" t="s">
         <v>74</v>
       </c>
@@ -5754,8 +5748,8 @@
         <v>8</v>
       </c>
       <c r="F20" s="15"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="84"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="76"/>
       <c r="I20" s="12">
         <v>43654</v>
       </c>
@@ -5763,15 +5757,15 @@
         <v>43654</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L20" s="7" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:12" s="1" customFormat="1">
-      <c r="B21" s="81"/>
-      <c r="C21" s="86"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="15" t="s">
         <v>76</v>
       </c>
@@ -5779,8 +5773,8 @@
         <v>16</v>
       </c>
       <c r="F21" s="15"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="84"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="76"/>
       <c r="I21" s="12">
         <v>43654</v>
       </c>
@@ -5795,8 +5789,8 @@
       </c>
     </row>
     <row r="22" spans="2:12" s="1" customFormat="1">
-      <c r="B22" s="81"/>
-      <c r="C22" s="86"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="15" t="s">
         <v>78</v>
       </c>
@@ -5804,8 +5798,8 @@
         <v>16</v>
       </c>
       <c r="F22" s="15"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="84"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="76"/>
       <c r="I22" s="12">
         <v>43655</v>
       </c>
@@ -5813,15 +5807,15 @@
         <v>43655</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L22" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:12" s="1" customFormat="1">
-      <c r="B23" s="81"/>
-      <c r="C23" s="86"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="15" t="s">
         <v>80</v>
       </c>
@@ -5829,8 +5823,8 @@
         <v>16</v>
       </c>
       <c r="F23" s="15"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="84"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="76"/>
       <c r="I23" s="12">
         <v>43655</v>
       </c>
@@ -5845,8 +5839,8 @@
       </c>
     </row>
     <row r="24" spans="2:12" s="1" customFormat="1" ht="25.5">
-      <c r="B24" s="81"/>
-      <c r="C24" s="86"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="15" t="s">
         <v>82</v>
       </c>
@@ -5854,8 +5848,8 @@
         <v>20</v>
       </c>
       <c r="F24" s="15"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="84"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="76"/>
       <c r="I24" s="12">
         <v>43656</v>
       </c>
@@ -5870,8 +5864,8 @@
       </c>
     </row>
     <row r="25" spans="2:12" s="1" customFormat="1">
-      <c r="B25" s="81"/>
-      <c r="C25" s="86"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="15" t="s">
         <v>84</v>
       </c>
@@ -5879,8 +5873,8 @@
         <v>20</v>
       </c>
       <c r="F25" s="15"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="85"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="77"/>
       <c r="I25" s="12">
         <v>43657</v>
       </c>
@@ -5888,15 +5882,15 @@
         <v>43657</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L25" s="7" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:12" s="1" customFormat="1">
-      <c r="B26" s="81"/>
-      <c r="C26" s="76"/>
+      <c r="B26" s="82"/>
+      <c r="C26" s="86"/>
       <c r="D26" s="62" t="s">
         <v>108</v>
       </c>
@@ -5904,7 +5898,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="15"/>
-      <c r="G26" s="79"/>
+      <c r="G26" s="80"/>
       <c r="H26" s="57"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -5912,10 +5906,10 @@
       <c r="L26" s="7"/>
     </row>
     <row r="27" spans="2:12" s="1" customFormat="1" ht="38.25">
-      <c r="B27" s="81">
+      <c r="B27" s="82">
         <v>5</v>
       </c>
-      <c r="C27" s="75" t="s">
+      <c r="C27" s="84" t="s">
         <v>86</v>
       </c>
       <c r="D27" s="44" t="s">
@@ -5925,7 +5919,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="15"/>
-      <c r="G27" s="77" t="s">
+      <c r="G27" s="78" t="s">
         <v>88</v>
       </c>
       <c r="H27" s="53"/>
@@ -5936,15 +5930,15 @@
         <v>43664</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L27" s="50" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="28" spans="2:12" s="1" customFormat="1">
-      <c r="B28" s="82"/>
-      <c r="C28" s="76"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="86"/>
       <c r="D28" s="62" t="s">
         <v>109</v>
       </c>
@@ -5952,7 +5946,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="15"/>
-      <c r="G28" s="79"/>
+      <c r="G28" s="80"/>
       <c r="H28" s="57"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
@@ -6039,6 +6033,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="G14:G26"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="B14:B26"/>
+    <mergeCell ref="B27:B28"/>
     <mergeCell ref="H8:H25"/>
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="B8:B13"/>
@@ -6054,12 +6054,6 @@
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="L4:L5"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="G14:G26"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="B14:B26"/>
-    <mergeCell ref="B27:B28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L8" r:id="rId1" display="https://www.w3schools.com/js/default.asp" xr:uid="{00000000-0004-0000-0400-000000000000}"/>

</xml_diff>